<commit_message>
done thietbi and quanlythietbi
</commit_message>
<xml_diff>
--- a/DanhSachSinhVien.xlsx
+++ b/DanhSachSinhVien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
   <si>
     <t>STT</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Địa Chỉ</t>
   </si>
   <si>
-    <t>Ngành Sinh</t>
+    <t>Ngày Sinh</t>
   </si>
   <si>
     <t>Ngành</t>
@@ -47,7 +47,7 @@
     <t>Ngày Vào</t>
   </si>
   <si>
-    <t>Mà Phòng</t>
+    <t>Mã Phòng</t>
   </si>
   <si>
     <t>Số Lần Vi Phạm</t>
@@ -56,232 +56,214 @@
     <t>Trạng Thái</t>
   </si>
   <si>
-    <t>C2002000</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\1_ptnanh_B2.jpg</t>
-  </si>
-  <si>
-    <t>Phạm Thị Nhật Anh</t>
-  </si>
-  <si>
-    <t>0777241111</t>
+    <t>C2002001</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\2_ntmcam_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Mỹ Cẩm</t>
+  </si>
+  <si>
+    <t>0777241999</t>
   </si>
   <si>
     <t>Nữ</t>
   </si>
   <si>
+    <t>Phú Dương, Tp Huế</t>
+  </si>
+  <si>
+    <t>1999-06-10</t>
+  </si>
+  <si>
+    <t>QLDU&amp;LT</t>
+  </si>
+  <si>
+    <t>K17</t>
+  </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
+  <si>
+    <t>Đang Thuê</t>
+  </si>
+  <si>
+    <t>C2002002</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\3_tttdung_B2.jpg</t>
+  </si>
+  <si>
+    <t>Trần Thị Thuỳ Dung</t>
+  </si>
+  <si>
+    <t>0777241113</t>
+  </si>
+  <si>
+    <t>Phú Thuận, Phú Vang</t>
+  </si>
+  <si>
+    <t>1999-06-01</t>
+  </si>
+  <si>
+    <t>NNT</t>
+  </si>
+  <si>
+    <t>K18</t>
+  </si>
+  <si>
+    <t>2022-01-20</t>
+  </si>
+  <si>
+    <t>C2002003</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\4_nvxdai_B2.JPG</t>
+  </si>
+  <si>
+    <t>Nguyễn Võ Xuân Đài</t>
+  </si>
+  <si>
+    <t>0777241114</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Phú Dương, TP Huế</t>
+  </si>
+  <si>
+    <t>1999-06-09</t>
+  </si>
+  <si>
+    <t>KTOT</t>
+  </si>
+  <si>
+    <t>2022-01-11</t>
+  </si>
+  <si>
+    <t>C2002004</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\5_nmguyn_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Guyn</t>
+  </si>
+  <si>
+    <t>0777241115</t>
+  </si>
+  <si>
+    <t>Thuận An, Tp Huế</t>
+  </si>
+  <si>
+    <t>C2002005</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\6_ntthao_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Thanh Thảo</t>
+  </si>
+  <si>
+    <t>0777241116</t>
+  </si>
+  <si>
+    <t>1999-06-04</t>
+  </si>
+  <si>
+    <t>C2002006</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\7_ntdhien_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Diệu Hiền</t>
+  </si>
+  <si>
+    <t>0777241117</t>
+  </si>
+  <si>
+    <t>Phú Mậu, Tp Huế</t>
+  </si>
+  <si>
+    <t>1999-06-03</t>
+  </si>
+  <si>
+    <t>NNA</t>
+  </si>
+  <si>
+    <t>2022-01-05</t>
+  </si>
+  <si>
+    <t>C2002007</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\8_ntahoa_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Ái Hoa</t>
+  </si>
+  <si>
+    <t>0777241118</t>
+  </si>
+  <si>
+    <t>Phú Thượng, Tp Huế</t>
+  </si>
+  <si>
+    <t>C2002008</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\9_ndhoang_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Đắc Hoàng</t>
+  </si>
+  <si>
+    <t>2022-01-16</t>
+  </si>
+  <si>
+    <t>C2002009</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\10_ptdhue_B2.jpg</t>
+  </si>
+  <si>
+    <t>Phùng Thị Diệu Huê</t>
+  </si>
+  <si>
+    <t>C2002010</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\11_nthung_B2.jpg</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Hùng</t>
+  </si>
+  <si>
+    <t>0981059000</t>
+  </si>
+  <si>
+    <t>Phú Xuân, Phú Vang</t>
+  </si>
+  <si>
+    <t>1999-05-12</t>
+  </si>
+  <si>
+    <t>2022-01-10</t>
+  </si>
+  <si>
+    <t>C2002011</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\12B2\12_ptkkieu_B2.jpg</t>
+  </si>
+  <si>
+    <t>Phạm Thị Kim Kiều</t>
+  </si>
+  <si>
     <t>Phú Mậu, TP Huế</t>
-  </si>
-  <si>
-    <t>1999-06-15</t>
-  </si>
-  <si>
-    <t>NNA</t>
-  </si>
-  <si>
-    <t>K18</t>
-  </si>
-  <si>
-    <t>2022-01-09</t>
-  </si>
-  <si>
-    <t>Đang Thuê</t>
-  </si>
-  <si>
-    <t>C2002001</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\2_ntmcam_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Mỹ Cẩm</t>
-  </si>
-  <si>
-    <t>0777241999</t>
-  </si>
-  <si>
-    <t>Phú Dương, Tp Huế</t>
-  </si>
-  <si>
-    <t>1999-06-10</t>
-  </si>
-  <si>
-    <t>QLDU&amp;LT</t>
-  </si>
-  <si>
-    <t>K17</t>
-  </si>
-  <si>
-    <t>2022-01-19</t>
-  </si>
-  <si>
-    <t>C2002002</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\3_tttdung_B2.jpg</t>
-  </si>
-  <si>
-    <t>Trần Thị Thuỳ Dung</t>
-  </si>
-  <si>
-    <t>0777241113</t>
-  </si>
-  <si>
-    <t>Phú Thuận, Phú Vang</t>
-  </si>
-  <si>
-    <t>1999-06-01</t>
-  </si>
-  <si>
-    <t>NNT</t>
-  </si>
-  <si>
-    <t>2022-01-20</t>
-  </si>
-  <si>
-    <t>C2002003</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\4_nvxdai_B2.JPG</t>
-  </si>
-  <si>
-    <t>Nguyễn Võ Xuân Đài</t>
-  </si>
-  <si>
-    <t>0777241114</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>Phú Dương, TP Huế</t>
-  </si>
-  <si>
-    <t>1999-06-09</t>
-  </si>
-  <si>
-    <t>KTOT</t>
-  </si>
-  <si>
-    <t>2022-01-11</t>
-  </si>
-  <si>
-    <t>C2002004</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\5_nmguyn_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Guyn</t>
-  </si>
-  <si>
-    <t>0777241115</t>
-  </si>
-  <si>
-    <t>Thuận An, Tp Huế</t>
-  </si>
-  <si>
-    <t>C2002005</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\6_ntthao_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Thanh Thảo</t>
-  </si>
-  <si>
-    <t>0777241116</t>
-  </si>
-  <si>
-    <t>1999-06-04</t>
-  </si>
-  <si>
-    <t>C2002006</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\7_ntdhien_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Diệu Hiền</t>
-  </si>
-  <si>
-    <t>0777241117</t>
-  </si>
-  <si>
-    <t>Phú Mậu, Tp Huế</t>
-  </si>
-  <si>
-    <t>1999-06-03</t>
-  </si>
-  <si>
-    <t>2022-01-05</t>
-  </si>
-  <si>
-    <t>C2002007</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\8_ntahoa_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Ái Hoa</t>
-  </si>
-  <si>
-    <t>0777241118</t>
-  </si>
-  <si>
-    <t>Phú Thượng, Tp Huế</t>
-  </si>
-  <si>
-    <t>C2002008</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\9_ndhoang_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Đắc Hoàng</t>
-  </si>
-  <si>
-    <t>2022-01-16</t>
-  </si>
-  <si>
-    <t>C2002009</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\10_ptdhue_B2.jpg</t>
-  </si>
-  <si>
-    <t>Phùng Thị Diệu Huê</t>
-  </si>
-  <si>
-    <t>C2002010</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\11_nthung_B2.jpg</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Hùng</t>
-  </si>
-  <si>
-    <t>0981059000</t>
-  </si>
-  <si>
-    <t>Phú Xuân, Phú Vang</t>
-  </si>
-  <si>
-    <t>1999-05-12</t>
-  </si>
-  <si>
-    <t>2022-01-10</t>
-  </si>
-  <si>
-    <t>C2002011</t>
-  </si>
-  <si>
-    <t>C:\Users\Admin\Desktop\12B2\12_ptkkieu_B2.jpg</t>
-  </si>
-  <si>
-    <t>Phạm Thị Kim Kiều</t>
   </si>
   <si>
     <t>1999-05-11</t>
@@ -389,98 +371,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A2:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -488,40 +426,40 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="L3" t="n">
         <v>100.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
@@ -532,34 +470,34 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="L4" t="n">
         <v>102.0</v>
@@ -576,34 +514,34 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>50</v>
       </c>
       <c r="L5" t="n">
         <v>100.0</v>
@@ -620,34 +558,34 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="L6" t="n">
         <v>100.0</v>
@@ -664,34 +602,34 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L7" t="n">
         <v>102.0</v>
@@ -708,34 +646,34 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L8" t="n">
         <v>101.0</v>
@@ -752,34 +690,34 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="L9" t="n">
         <v>100.0</v>
@@ -796,34 +734,34 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="L10" t="n">
         <v>101.0</v>
@@ -840,34 +778,34 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="L11" t="n">
         <v>100.0</v>
@@ -884,34 +822,34 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K12" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L12" t="n">
         <v>102.0</v>
@@ -928,34 +866,34 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L13" t="n">
         <v>100.0</v>
@@ -972,34 +910,34 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="L14" t="n">
         <v>102.0</v>
@@ -1016,34 +954,34 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K15" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="L15" t="n">
         <v>101.0</v>
@@ -1060,34 +998,34 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L16" t="n">
         <v>100.0</v>
@@ -1104,34 +1042,34 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I17" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="L17" t="n">
         <v>101.0</v>

</xml_diff>